<commit_message>
Updated UI: Enhanced design for dashboard, register and index pages
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test3@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Subhadra Mahato</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>